<commit_message>
Instalacion de Librerias con Freeze
</commit_message>
<xml_diff>
--- a/excelFile.xlsx
+++ b/excelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Desktop\Proyecto Invitaciones Evento\evento-gestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB23530-4067-4972-B327-D54AE084BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5C705-2EF1-41AA-8CC6-3877CD0AD1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16770" windowHeight="9315" xr2:uid="{FE98FE93-B088-4AD3-820F-6EA189EB7DCB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FE98FE93-B088-4AD3-820F-6EA189EB7DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Frase</t>
+  </si>
+  <si>
+    <t>6 Boletos</t>
+  </si>
+  <si>
+    <t>7 Boletos</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +496,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -501,7 +507,7 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">

</xml_diff>